<commit_message>
fix: :card_file_box: FIX DATA 2014
</commit_message>
<xml_diff>
--- a/apps/load_data/2014/02/PLMOVMAE.xlsx
+++ b/apps/load_data/2014/02/PLMOVMAE.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2014\HHY0214\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HHY ACTUALIZADOS\2014\HHY0214\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D9E3A9F-E866-4A3B-A837-473BAC70B9B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7070E4DF-4006-44F9-B72B-0F173A321919}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12645" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12645" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLMOVMAE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLMOVMAE!$A$1:$CF$224</definedName>
     <definedName name="_xlnm.Database">PLMOVMAE!$A$1:$CF$224</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9335" uniqueCount="2300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9337" uniqueCount="2299">
   <si>
     <t>CODEJE</t>
   </si>
@@ -6314,9 +6315,6 @@
   </si>
   <si>
     <t>048561</t>
-  </si>
-  <si>
-    <t>RD-456-2010-HNHU</t>
   </si>
   <si>
     <t>1001      500000000000001002      378000000000001005         400000000001007       50100000000001021     2150600000000001022     2494700000000001031     2893800000000001033    13012700000000001039     6200000000000001042     300000000000000</t>
@@ -6928,7 +6926,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -7409,11 +7407,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7768,10 +7770,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q236" sqref="Q236"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7785,33 +7789,32 @@
     <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="4.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="33.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="1.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="8.7109375" style="1" customWidth="1"/>
     <col min="15" max="15" width="1.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="1.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="2.7109375" style="1" customWidth="1"/>
     <col min="24" max="24" width="1.7109375" style="1" customWidth="1"/>
     <col min="25" max="25" width="3.7109375" style="1" customWidth="1"/>
     <col min="26" max="26" width="4.7109375" style="2" customWidth="1"/>
     <col min="27" max="27" width="3.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="15.7109375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="8.7109375" customWidth="1"/>
-    <col min="30" max="30" width="16.7109375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" customWidth="1"/>
+    <col min="30" max="30" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.7109375" customWidth="1"/>
     <col min="32" max="32" width="3.7109375" style="1" customWidth="1"/>
     <col min="33" max="33" width="4.7109375" style="1" customWidth="1"/>
     <col min="34" max="34" width="2.7109375" style="1" customWidth="1"/>
     <col min="35" max="36" width="1.7109375" style="1" customWidth="1"/>
     <col min="37" max="39" width="2.7109375" style="1" customWidth="1"/>
-    <col min="40" max="40" width="25.7109375" style="1" customWidth="1"/>
+    <col min="40" max="40" width="9" style="1" customWidth="1"/>
     <col min="41" max="41" width="3.7109375" style="1" customWidth="1"/>
     <col min="42" max="43" width="1.7109375" style="1" customWidth="1"/>
     <col min="44" max="45" width="2.7109375" style="1" customWidth="1"/>
@@ -41824,6 +41827,9 @@
       <c r="AB189" s="1" t="s">
         <v>1793</v>
       </c>
+      <c r="AD189" s="1" t="s">
+        <v>2078</v>
+      </c>
       <c r="AF189" s="1" t="s">
         <v>104</v>
       </c>
@@ -42006,6 +42012,9 @@
       <c r="AC190" s="3">
         <v>36869</v>
       </c>
+      <c r="AD190" s="1" t="s">
+        <v>2078</v>
+      </c>
       <c r="AF190" s="1" t="s">
         <v>104</v>
       </c>
@@ -42182,6 +42191,9 @@
       <c r="AC191" s="3">
         <v>37453</v>
       </c>
+      <c r="AD191" s="1" t="s">
+        <v>2078</v>
+      </c>
       <c r="AF191" s="1" t="s">
         <v>104</v>
       </c>
@@ -42464,7 +42476,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="193" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>84</v>
       </c>
@@ -42649,7 +42661,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="194" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>84</v>
       </c>
@@ -42825,7 +42837,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="195" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>84</v>
       </c>
@@ -42995,7 +43007,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="196" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>84</v>
       </c>
@@ -43153,7 +43165,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="197" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>84</v>
       </c>
@@ -43311,7 +43323,7 @@
         <v>2086</v>
       </c>
     </row>
-    <row r="198" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>84</v>
       </c>
@@ -43469,7 +43481,7 @@
         <v>2091</v>
       </c>
     </row>
-    <row r="199" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>84</v>
       </c>
@@ -43627,195 +43639,211 @@
         <v>312</v>
       </c>
     </row>
-    <row r="200" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
+    <row r="200" spans="1:84" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B200" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="C200" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D200" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="E200" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="F200" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G200" s="1" t="s">
+      <c r="F200" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G200" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H200" s="1" t="s">
+      <c r="H200" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I200" s="1" t="s">
+      <c r="I200" s="4" t="s">
         <v>2095</v>
       </c>
-      <c r="J200" s="1" t="s">
+      <c r="J200" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K200" s="1" t="s">
+      <c r="K200" s="4" t="s">
         <v>1570</v>
       </c>
-      <c r="L200" s="1" t="s">
+      <c r="L200" s="4" t="s">
         <v>2096</v>
       </c>
-      <c r="M200" s="1" t="s">
+      <c r="M200" s="4" t="s">
         <v>1992</v>
       </c>
-      <c r="N200" s="1" t="s">
+      <c r="N200" s="4" t="s">
         <v>1572</v>
       </c>
-      <c r="Q200" s="3">
+      <c r="O200" s="4"/>
+      <c r="P200" s="4"/>
+      <c r="Q200" s="5">
         <v>20980</v>
       </c>
-      <c r="R200" s="1" t="s">
+      <c r="R200" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="S200" s="3">
+      <c r="S200" s="5">
         <v>38078</v>
       </c>
-      <c r="T200" s="1" t="s">
+      <c r="T200" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="V200" s="1" t="s">
+      <c r="V200" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Y200" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z200" s="2">
+      <c r="W200" s="4"/>
+      <c r="X200" s="4"/>
+      <c r="Y200" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z200" s="7">
         <v>20</v>
       </c>
-      <c r="AA200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB200" s="1" t="s">
+      <c r="AA200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB200" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="AC200" s="3">
-        <v>40544</v>
-      </c>
-      <c r="AD200" s="1" t="s">
+      <c r="AC200" s="5"/>
+      <c r="AD200" s="4"/>
+      <c r="AF200" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG200" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="AH200" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI200" s="4"/>
+      <c r="AJ200" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN200" s="4"/>
+      <c r="AO200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP200" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ200" s="4"/>
+      <c r="AR200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV200" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW200" s="4"/>
+      <c r="AX200" s="4"/>
+      <c r="AY200" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AZ200" s="4" t="s">
+        <v>1573</v>
+      </c>
+      <c r="BA200" s="4"/>
+      <c r="BB200" s="4">
+        <v>8</v>
+      </c>
+      <c r="BC200" s="4">
+        <v>11</v>
+      </c>
+      <c r="BD200" s="4"/>
+      <c r="BE200" s="4"/>
+      <c r="BF200" s="4"/>
+      <c r="BG200" s="4"/>
+      <c r="BH200" s="4" t="s">
         <v>2097</v>
       </c>
-      <c r="AF200" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG200" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="AH200" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="AJ200" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP200" s="1" t="s">
+      <c r="BI200" s="4" t="s">
+        <v>2098</v>
+      </c>
+      <c r="BJ200" s="4" t="s">
+        <v>2099</v>
+      </c>
+      <c r="BK200" s="4"/>
+      <c r="BL200" s="4"/>
+      <c r="BM200" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="BN200" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="BO200" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BP200" s="4"/>
+      <c r="BQ200" s="4"/>
+      <c r="BR200" s="4" t="s">
+        <v>1576</v>
+      </c>
+      <c r="BS200" s="5">
+        <v>38132</v>
+      </c>
+      <c r="BT200" s="4" t="s">
+        <v>1577</v>
+      </c>
+      <c r="BU200" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="BV200" s="4"/>
+      <c r="BW200" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="BX200" s="4">
+        <v>0</v>
+      </c>
+      <c r="BY200" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AR200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV200" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY200" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ200" s="1" t="s">
-        <v>1573</v>
-      </c>
-      <c r="BB200" s="1">
-        <v>8</v>
-      </c>
-      <c r="BC200" s="1">
-        <v>11</v>
-      </c>
-      <c r="BH200" s="1" t="s">
-        <v>2098</v>
-      </c>
-      <c r="BI200" s="1" t="s">
-        <v>2099</v>
-      </c>
-      <c r="BJ200" s="1" t="s">
+      <c r="BZ200" s="4" t="s">
         <v>2100</v>
       </c>
-      <c r="BM200" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BN200" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BO200" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="BR200" s="1" t="s">
-        <v>1576</v>
-      </c>
-      <c r="BS200" s="3">
-        <v>38132</v>
-      </c>
-      <c r="BT200" s="1" t="s">
-        <v>1577</v>
-      </c>
-      <c r="BU200" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BW200" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="BX200" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY200" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BZ200" s="1" t="s">
-        <v>2101</v>
-      </c>
-      <c r="CA200" s="1" t="s">
+      <c r="CA200" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="CB200" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CC200" s="1" t="s">
+      <c r="CB200" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="CC200" s="4" t="s">
         <v>1578</v>
       </c>
-      <c r="CD200" s="1" t="s">
+      <c r="CD200" s="4" t="s">
         <v>1579</v>
       </c>
-      <c r="CE200" s="1" t="s">
+      <c r="CE200" s="4" t="s">
         <v>1580</v>
       </c>
+      <c r="CF200" s="4"/>
     </row>
-    <row r="201" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>84</v>
       </c>
@@ -43847,16 +43875,16 @@
         <v>93</v>
       </c>
       <c r="K201" s="1" t="s">
+        <v>2101</v>
+      </c>
+      <c r="L201" s="1" t="s">
         <v>2102</v>
-      </c>
-      <c r="L201" s="1" t="s">
-        <v>2103</v>
       </c>
       <c r="M201" s="1" t="s">
         <v>1992</v>
       </c>
       <c r="N201" s="1" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="Q201" s="3">
         <v>20242</v>
@@ -43889,7 +43917,7 @@
         <v>40726</v>
       </c>
       <c r="AD201" s="1" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="AF201" s="1" t="s">
         <v>263</v>
@@ -43937,13 +43965,13 @@
         <v>98</v>
       </c>
       <c r="AZ201" s="1" t="s">
+        <v>2105</v>
+      </c>
+      <c r="BH201" s="1" t="s">
         <v>2106</v>
       </c>
-      <c r="BH201" s="1" t="s">
+      <c r="BI201" s="1" t="s">
         <v>2107</v>
-      </c>
-      <c r="BI201" s="1" t="s">
-        <v>2108</v>
       </c>
       <c r="BM201" s="1" t="s">
         <v>115</v>
@@ -43955,13 +43983,13 @@
         <v>217</v>
       </c>
       <c r="BR201" s="1" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="BS201" s="3">
         <v>34200</v>
       </c>
       <c r="BT201" s="1" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="BU201" s="1" t="s">
         <v>119</v>
@@ -43988,10 +44016,10 @@
         <v>123</v>
       </c>
       <c r="CE201" s="1" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
     </row>
-    <row r="202" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>84</v>
       </c>
@@ -44017,22 +44045,22 @@
         <v>91</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="J202" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K202" s="1" t="s">
+        <v>2112</v>
+      </c>
+      <c r="L202" s="1" t="s">
         <v>2113</v>
-      </c>
-      <c r="L202" s="1" t="s">
-        <v>2114</v>
       </c>
       <c r="M202" s="1" t="s">
         <v>1992</v>
       </c>
       <c r="N202" s="1" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="Q202" s="3">
         <v>27336</v>
@@ -44065,7 +44093,7 @@
         <v>41244</v>
       </c>
       <c r="AD202" s="1" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="AF202" s="1" t="s">
         <v>104</v>
@@ -44113,13 +44141,13 @@
         <v>98</v>
       </c>
       <c r="AZ202" s="1" t="s">
+        <v>2116</v>
+      </c>
+      <c r="BH202" s="1" t="s">
+        <v>2097</v>
+      </c>
+      <c r="BI202" s="1" t="s">
         <v>2117</v>
-      </c>
-      <c r="BH202" s="1" t="s">
-        <v>2098</v>
-      </c>
-      <c r="BI202" s="1" t="s">
-        <v>2118</v>
       </c>
       <c r="BM202" s="1" t="s">
         <v>115</v>
@@ -44131,13 +44159,13 @@
         <v>116</v>
       </c>
       <c r="BR202" s="1" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="BS202" s="3">
         <v>36347</v>
       </c>
       <c r="BT202" s="1" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="BU202" s="1" t="s">
         <v>119</v>
@@ -44152,7 +44180,7 @@
         <v>108</v>
       </c>
       <c r="BZ202" s="1" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="CA202" s="1" t="s">
         <v>121</v>
@@ -44161,16 +44189,16 @@
         <v>98</v>
       </c>
       <c r="CC202" s="1" t="s">
+        <v>2121</v>
+      </c>
+      <c r="CD202" s="1" t="s">
         <v>2122</v>
       </c>
-      <c r="CD202" s="1" t="s">
+      <c r="CE202" s="1" t="s">
         <v>2123</v>
       </c>
-      <c r="CE202" s="1" t="s">
-        <v>2124</v>
-      </c>
     </row>
-    <row r="203" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>84</v>
       </c>
@@ -44202,16 +44230,16 @@
         <v>93</v>
       </c>
       <c r="K203" s="1" t="s">
+        <v>2124</v>
+      </c>
+      <c r="L203" s="1" t="s">
         <v>2125</v>
-      </c>
-      <c r="L203" s="1" t="s">
-        <v>2126</v>
       </c>
       <c r="M203" s="1" t="s">
         <v>1992</v>
       </c>
       <c r="N203" s="1" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="Q203" s="3">
         <v>21430</v>
@@ -44247,7 +44275,7 @@
         <v>41330</v>
       </c>
       <c r="AD203" s="1" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="AF203" s="1" t="s">
         <v>104</v>
@@ -44298,10 +44326,10 @@
         <v>98</v>
       </c>
       <c r="BH203" s="1" t="s">
+        <v>2128</v>
+      </c>
+      <c r="BI203" s="1" t="s">
         <v>2129</v>
-      </c>
-      <c r="BI203" s="1" t="s">
-        <v>2130</v>
       </c>
       <c r="BM203" s="1" t="s">
         <v>115</v>
@@ -44310,7 +44338,7 @@
         <v>103</v>
       </c>
       <c r="BT203" s="1" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="BU203" s="1" t="s">
         <v>119</v>
@@ -44334,16 +44362,16 @@
         <v>98</v>
       </c>
       <c r="CC203" s="1" t="s">
+        <v>2131</v>
+      </c>
+      <c r="CD203" s="1" t="s">
         <v>2132</v>
       </c>
-      <c r="CD203" s="1" t="s">
+      <c r="CE203" s="1" t="s">
         <v>2133</v>
       </c>
-      <c r="CE203" s="1" t="s">
-        <v>2134</v>
-      </c>
     </row>
-    <row r="204" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>84</v>
       </c>
@@ -44375,16 +44403,16 @@
         <v>93</v>
       </c>
       <c r="K204" s="1" t="s">
+        <v>2124</v>
+      </c>
+      <c r="L204" s="1" t="s">
         <v>2125</v>
-      </c>
-      <c r="L204" s="1" t="s">
-        <v>2126</v>
       </c>
       <c r="M204" s="1" t="s">
         <v>1992</v>
       </c>
       <c r="N204" s="1" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="Q204" s="3">
         <v>21430</v>
@@ -44420,7 +44448,7 @@
         <v>41330</v>
       </c>
       <c r="AD204" s="1" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="AF204" s="1" t="s">
         <v>104</v>
@@ -44471,10 +44499,10 @@
         <v>98</v>
       </c>
       <c r="BH204" s="1" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="BI204" s="1" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="BM204" s="1" t="s">
         <v>115</v>
@@ -44483,7 +44511,7 @@
         <v>103</v>
       </c>
       <c r="BT204" s="1" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="BU204" s="1" t="s">
         <v>119</v>
@@ -44507,16 +44535,16 @@
         <v>98</v>
       </c>
       <c r="CC204" s="1" t="s">
+        <v>2131</v>
+      </c>
+      <c r="CD204" s="1" t="s">
         <v>2132</v>
       </c>
-      <c r="CD204" s="1" t="s">
+      <c r="CE204" s="1" t="s">
         <v>2133</v>
       </c>
-      <c r="CE204" s="1" t="s">
-        <v>2134</v>
-      </c>
     </row>
-    <row r="205" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>84</v>
       </c>
@@ -44548,16 +44576,16 @@
         <v>93</v>
       </c>
       <c r="K205" s="1" t="s">
+        <v>2135</v>
+      </c>
+      <c r="L205" s="1" t="s">
         <v>2136</v>
-      </c>
-      <c r="L205" s="1" t="s">
-        <v>2137</v>
       </c>
       <c r="M205" s="1" t="s">
         <v>1992</v>
       </c>
       <c r="N205" s="1" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="Q205" s="3">
         <v>21965</v>
@@ -44587,13 +44615,13 @@
         <v>0</v>
       </c>
       <c r="AB205" s="1" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="AC205" s="3">
         <v>41579</v>
       </c>
       <c r="AD205" s="1" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="AF205" s="1" t="s">
         <v>104</v>
@@ -44641,13 +44669,13 @@
         <v>98</v>
       </c>
       <c r="AZ205" s="1" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="BD205" s="1" t="s">
         <v>99</v>
       </c>
       <c r="BH205" s="1" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="BM205" s="1" t="s">
         <v>115</v>
@@ -44659,13 +44687,13 @@
         <v>217</v>
       </c>
       <c r="BR205" s="1" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="BS205" s="3">
         <v>35087</v>
       </c>
       <c r="BT205" s="1" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="BU205" s="1" t="s">
         <v>119</v>
@@ -44686,16 +44714,16 @@
         <v>98</v>
       </c>
       <c r="CC205" s="1" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="CD205" s="1" t="s">
         <v>1624</v>
       </c>
       <c r="CE205" s="1" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
     </row>
-    <row r="206" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>84</v>
       </c>
@@ -44727,13 +44755,13 @@
         <v>93</v>
       </c>
       <c r="K206" s="1" t="s">
+        <v>2146</v>
+      </c>
+      <c r="L206" s="1" t="s">
         <v>2147</v>
       </c>
-      <c r="L206" s="1" t="s">
+      <c r="N206" s="1" t="s">
         <v>2148</v>
-      </c>
-      <c r="N206" s="1" t="s">
-        <v>2149</v>
       </c>
       <c r="O206" s="1" t="s">
         <v>97</v>
@@ -44811,7 +44839,7 @@
         <v>98</v>
       </c>
       <c r="AZ206" s="1" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="BB206" s="1">
         <v>2</v>
@@ -44829,10 +44857,10 @@
         <v>112</v>
       </c>
       <c r="BH206" s="1" t="s">
+        <v>2150</v>
+      </c>
+      <c r="BI206" s="1" t="s">
         <v>2151</v>
-      </c>
-      <c r="BI206" s="1" t="s">
-        <v>2152</v>
       </c>
       <c r="BM206" s="1" t="s">
         <v>115</v>
@@ -44844,13 +44872,13 @@
         <v>217</v>
       </c>
       <c r="BR206" s="1" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="BS206" s="3">
         <v>39189</v>
       </c>
       <c r="BT206" s="1" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="BU206" s="1" t="s">
         <v>119</v>
@@ -44877,13 +44905,13 @@
         <v>255</v>
       </c>
       <c r="CD206" s="1" t="s">
+        <v>2154</v>
+      </c>
+      <c r="CE206" s="1" t="s">
         <v>2155</v>
       </c>
-      <c r="CE206" s="1" t="s">
-        <v>2156</v>
-      </c>
     </row>
-    <row r="207" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>84</v>
       </c>
@@ -44915,13 +44943,13 @@
         <v>93</v>
       </c>
       <c r="K207" s="1" t="s">
+        <v>2156</v>
+      </c>
+      <c r="L207" s="1" t="s">
         <v>2157</v>
       </c>
-      <c r="L207" s="1" t="s">
+      <c r="N207" s="1" t="s">
         <v>2158</v>
-      </c>
-      <c r="N207" s="1" t="s">
-        <v>2159</v>
       </c>
       <c r="O207" s="1" t="s">
         <v>97</v>
@@ -45002,7 +45030,7 @@
         <v>98</v>
       </c>
       <c r="AZ207" s="1" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="BB207" s="1">
         <v>2</v>
@@ -45020,7 +45048,7 @@
         <v>112</v>
       </c>
       <c r="BH207" s="1" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="BM207" s="1" t="s">
         <v>115</v>
@@ -45032,13 +45060,13 @@
         <v>99</v>
       </c>
       <c r="BR207" s="1" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="BS207" s="3">
         <v>37286</v>
       </c>
       <c r="BT207" s="1" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="BU207" s="1" t="s">
         <v>119</v>
@@ -45068,10 +45096,10 @@
         <v>2070</v>
       </c>
       <c r="CE207" s="1" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
     </row>
-    <row r="208" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>84</v>
       </c>
@@ -45103,13 +45131,13 @@
         <v>93</v>
       </c>
       <c r="K208" s="1" t="s">
+        <v>2164</v>
+      </c>
+      <c r="L208" s="1" t="s">
         <v>2165</v>
       </c>
-      <c r="L208" s="1" t="s">
+      <c r="N208" s="1" t="s">
         <v>2166</v>
-      </c>
-      <c r="N208" s="1" t="s">
-        <v>2167</v>
       </c>
       <c r="O208" s="1" t="s">
         <v>97</v>
@@ -45190,7 +45218,7 @@
         <v>98</v>
       </c>
       <c r="AZ208" s="1" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="BB208" s="1">
         <v>2</v>
@@ -45208,7 +45236,7 @@
         <v>112</v>
       </c>
       <c r="BH208" s="1" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="BM208" s="1" t="s">
         <v>115</v>
@@ -45220,13 +45248,13 @@
         <v>217</v>
       </c>
       <c r="BR208" s="1" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="BS208" s="3">
         <v>37421</v>
       </c>
       <c r="BT208" s="1" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="BU208" s="1" t="s">
         <v>119</v>
@@ -45250,13 +45278,13 @@
         <v>98</v>
       </c>
       <c r="CC208" s="1" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="CD208" s="1" t="s">
         <v>520</v>
       </c>
       <c r="CE208" s="1" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="209" spans="1:83" x14ac:dyDescent="0.25">
@@ -45273,7 +45301,7 @@
         <v>208</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>98</v>
@@ -45285,19 +45313,19 @@
         <v>91</v>
       </c>
       <c r="I209" s="1" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="J209" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K209" s="1" t="s">
+        <v>2175</v>
+      </c>
+      <c r="L209" s="1" t="s">
         <v>2176</v>
       </c>
-      <c r="L209" s="1" t="s">
+      <c r="N209" s="1" t="s">
         <v>2177</v>
-      </c>
-      <c r="N209" s="1" t="s">
-        <v>2178</v>
       </c>
       <c r="O209" s="1" t="s">
         <v>97</v>
@@ -45381,7 +45409,7 @@
         <v>98</v>
       </c>
       <c r="AZ209" s="1" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="BB209" s="1">
         <v>2</v>
@@ -45408,7 +45436,7 @@
         <v>103</v>
       </c>
       <c r="BT209" s="1" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="BU209" s="1" t="s">
         <v>119</v>
@@ -45432,13 +45460,13 @@
         <v>98</v>
       </c>
       <c r="CC209" s="1" t="s">
+        <v>2180</v>
+      </c>
+      <c r="CD209" s="1" t="s">
         <v>2181</v>
       </c>
-      <c r="CD209" s="1" t="s">
+      <c r="CE209" s="1" t="s">
         <v>2182</v>
-      </c>
-      <c r="CE209" s="1" t="s">
-        <v>2183</v>
       </c>
     </row>
     <row r="210" spans="1:83" x14ac:dyDescent="0.25">
@@ -45473,13 +45501,13 @@
         <v>93</v>
       </c>
       <c r="K210" s="1" t="s">
+        <v>2183</v>
+      </c>
+      <c r="L210" s="1" t="s">
         <v>2184</v>
       </c>
-      <c r="L210" s="1" t="s">
+      <c r="N210" s="1" t="s">
         <v>2185</v>
-      </c>
-      <c r="N210" s="1" t="s">
-        <v>2186</v>
       </c>
       <c r="O210" s="1" t="s">
         <v>97</v>
@@ -45560,7 +45588,7 @@
         <v>98</v>
       </c>
       <c r="AZ210" s="1" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="BB210" s="1">
         <v>2</v>
@@ -45578,10 +45606,10 @@
         <v>112</v>
       </c>
       <c r="BH210" s="1" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="BI210" s="1" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="BM210" s="1" t="s">
         <v>115</v>
@@ -45593,13 +45621,13 @@
         <v>217</v>
       </c>
       <c r="BR210" s="1" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="BS210" s="3">
         <v>35215</v>
       </c>
       <c r="BT210" s="1" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="BU210" s="1" t="s">
         <v>119</v>
@@ -45623,13 +45651,13 @@
         <v>98</v>
       </c>
       <c r="CC210" s="1" t="s">
+        <v>2190</v>
+      </c>
+      <c r="CD210" s="1" t="s">
         <v>2191</v>
       </c>
-      <c r="CD210" s="1" t="s">
+      <c r="CE210" s="1" t="s">
         <v>2192</v>
-      </c>
-      <c r="CE210" s="1" t="s">
-        <v>2193</v>
       </c>
     </row>
     <row r="211" spans="1:83" x14ac:dyDescent="0.25">
@@ -45664,13 +45692,13 @@
         <v>93</v>
       </c>
       <c r="K211" s="1" t="s">
+        <v>2193</v>
+      </c>
+      <c r="L211" s="1" t="s">
         <v>2194</v>
       </c>
-      <c r="L211" s="1" t="s">
+      <c r="N211" s="1" t="s">
         <v>2195</v>
-      </c>
-      <c r="N211" s="1" t="s">
-        <v>2196</v>
       </c>
       <c r="O211" s="1" t="s">
         <v>97</v>
@@ -45754,7 +45782,7 @@
         <v>98</v>
       </c>
       <c r="AZ211" s="1" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="BB211" s="1">
         <v>2</v>
@@ -45772,7 +45800,7 @@
         <v>112</v>
       </c>
       <c r="BH211" s="1" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="BM211" s="1" t="s">
         <v>115</v>
@@ -45784,13 +45812,13 @@
         <v>217</v>
       </c>
       <c r="BR211" s="1" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="BS211" s="3">
         <v>35178</v>
       </c>
       <c r="BT211" s="1" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="BU211" s="1" t="s">
         <v>119</v>
@@ -45814,13 +45842,13 @@
         <v>89</v>
       </c>
       <c r="CC211" s="1" t="s">
+        <v>2200</v>
+      </c>
+      <c r="CD211" s="1" t="s">
         <v>2201</v>
       </c>
-      <c r="CD211" s="1" t="s">
+      <c r="CE211" s="1" t="s">
         <v>2202</v>
-      </c>
-      <c r="CE211" s="1" t="s">
-        <v>2203</v>
       </c>
     </row>
     <row r="212" spans="1:83" x14ac:dyDescent="0.25">
@@ -45855,13 +45883,13 @@
         <v>93</v>
       </c>
       <c r="K212" s="1" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="L212" s="1" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="N212" s="1" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="O212" s="1" t="s">
         <v>97</v>
@@ -45945,7 +45973,7 @@
         <v>98</v>
       </c>
       <c r="AZ212" s="1" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="BB212" s="1">
         <v>2</v>
@@ -45963,7 +45991,7 @@
         <v>112</v>
       </c>
       <c r="BH212" s="1" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="BM212" s="1" t="s">
         <v>115</v>
@@ -45972,13 +46000,13 @@
         <v>217</v>
       </c>
       <c r="BR212" s="1" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="BS212" s="3">
         <v>34200</v>
       </c>
       <c r="BT212" s="1" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="BU212" s="1" t="s">
         <v>119</v>
@@ -46008,7 +46036,7 @@
         <v>123</v>
       </c>
       <c r="CE212" s="1" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="213" spans="1:83" x14ac:dyDescent="0.25">
@@ -46016,10 +46044,10 @@
         <v>84</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>631</v>
@@ -46034,7 +46062,7 @@
         <v>90</v>
       </c>
       <c r="H213" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>631</v>
@@ -46043,13 +46071,13 @@
         <v>669</v>
       </c>
       <c r="K213" s="1" t="s">
+        <v>2208</v>
+      </c>
+      <c r="L213" s="1" t="s">
         <v>2209</v>
       </c>
-      <c r="L213" s="1" t="s">
+      <c r="N213" s="1" t="s">
         <v>2210</v>
-      </c>
-      <c r="N213" s="1" t="s">
-        <v>2211</v>
       </c>
       <c r="O213" s="1" t="s">
         <v>97</v>
@@ -46106,7 +46134,7 @@
         <v>0</v>
       </c>
       <c r="AN213" s="1" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="AO213" s="1">
         <v>0</v>
@@ -46151,13 +46179,13 @@
         <v>112</v>
       </c>
       <c r="BH213" s="1" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="BM213" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT213" s="1" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="BU213" s="1" t="s">
         <v>119</v>
@@ -46178,13 +46206,13 @@
         <v>98</v>
       </c>
       <c r="CC213" s="1" t="s">
+        <v>2214</v>
+      </c>
+      <c r="CD213" s="1" t="s">
         <v>2215</v>
       </c>
-      <c r="CD213" s="1" t="s">
+      <c r="CE213" s="1" t="s">
         <v>2216</v>
-      </c>
-      <c r="CE213" s="1" t="s">
-        <v>2217</v>
       </c>
     </row>
     <row r="214" spans="1:83" x14ac:dyDescent="0.25">
@@ -46192,10 +46220,10 @@
         <v>84</v>
       </c>
       <c r="B214" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C214" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>631</v>
@@ -46210,7 +46238,7 @@
         <v>90</v>
       </c>
       <c r="H214" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I214" s="1" t="s">
         <v>631</v>
@@ -46219,13 +46247,13 @@
         <v>669</v>
       </c>
       <c r="K214" s="1" t="s">
+        <v>2217</v>
+      </c>
+      <c r="L214" s="1" t="s">
         <v>2218</v>
       </c>
-      <c r="L214" s="1" t="s">
+      <c r="N214" s="1" t="s">
         <v>2219</v>
-      </c>
-      <c r="N214" s="1" t="s">
-        <v>2220</v>
       </c>
       <c r="O214" s="1" t="s">
         <v>97</v>
@@ -46279,7 +46307,7 @@
         <v>0</v>
       </c>
       <c r="AN214" s="1" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="AO214" s="1">
         <v>0</v>
@@ -46324,13 +46352,13 @@
         <v>112</v>
       </c>
       <c r="BH214" s="1" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="BM214" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT214" s="1" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="BU214" s="1" t="s">
         <v>119</v>
@@ -46357,7 +46385,7 @@
         <v>1097</v>
       </c>
       <c r="CE214" s="1" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="215" spans="1:83" x14ac:dyDescent="0.25">
@@ -46365,10 +46393,10 @@
         <v>84</v>
       </c>
       <c r="B215" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C215" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>631</v>
@@ -46383,7 +46411,7 @@
         <v>90</v>
       </c>
       <c r="H215" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>631</v>
@@ -46392,13 +46420,13 @@
         <v>669</v>
       </c>
       <c r="K215" s="1" t="s">
+        <v>2224</v>
+      </c>
+      <c r="L215" s="1" t="s">
         <v>2225</v>
       </c>
-      <c r="L215" s="1" t="s">
+      <c r="N215" s="1" t="s">
         <v>2226</v>
-      </c>
-      <c r="N215" s="1" t="s">
-        <v>2227</v>
       </c>
       <c r="O215" s="1" t="s">
         <v>97</v>
@@ -46452,7 +46480,7 @@
         <v>0</v>
       </c>
       <c r="AN215" s="1" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="AO215" s="1">
         <v>0</v>
@@ -46497,13 +46525,13 @@
         <v>112</v>
       </c>
       <c r="BH215" s="1" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="BM215" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT215" s="1" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="BU215" s="1" t="s">
         <v>119</v>
@@ -46524,13 +46552,13 @@
         <v>89</v>
       </c>
       <c r="CC215" s="1" t="s">
+        <v>2230</v>
+      </c>
+      <c r="CD215" s="1" t="s">
         <v>2231</v>
       </c>
-      <c r="CD215" s="1" t="s">
+      <c r="CE215" s="1" t="s">
         <v>2232</v>
-      </c>
-      <c r="CE215" s="1" t="s">
-        <v>2233</v>
       </c>
     </row>
     <row r="216" spans="1:83" x14ac:dyDescent="0.25">
@@ -46538,10 +46566,10 @@
         <v>84</v>
       </c>
       <c r="B216" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>631</v>
@@ -46556,7 +46584,7 @@
         <v>90</v>
       </c>
       <c r="H216" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I216" s="1" t="s">
         <v>631</v>
@@ -46565,13 +46593,13 @@
         <v>669</v>
       </c>
       <c r="K216" s="1" t="s">
+        <v>2233</v>
+      </c>
+      <c r="L216" s="1" t="s">
         <v>2234</v>
       </c>
-      <c r="L216" s="1" t="s">
+      <c r="N216" s="1" t="s">
         <v>2235</v>
-      </c>
-      <c r="N216" s="1" t="s">
-        <v>2236</v>
       </c>
       <c r="O216" s="1" t="s">
         <v>97</v>
@@ -46625,7 +46653,7 @@
         <v>0</v>
       </c>
       <c r="AN216" s="1" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="AO216" s="1">
         <v>0</v>
@@ -46670,13 +46698,13 @@
         <v>112</v>
       </c>
       <c r="BH216" s="1" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="BM216" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT216" s="1" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="BU216" s="1" t="s">
         <v>119</v>
@@ -46697,13 +46725,13 @@
         <v>89</v>
       </c>
       <c r="CC216" s="1" t="s">
+        <v>2239</v>
+      </c>
+      <c r="CD216" s="1" t="s">
         <v>2240</v>
       </c>
-      <c r="CD216" s="1" t="s">
+      <c r="CE216" s="1" t="s">
         <v>2241</v>
-      </c>
-      <c r="CE216" s="1" t="s">
-        <v>2242</v>
       </c>
     </row>
     <row r="217" spans="1:83" x14ac:dyDescent="0.25">
@@ -46711,10 +46739,10 @@
         <v>84</v>
       </c>
       <c r="B217" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C217" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>631</v>
@@ -46729,7 +46757,7 @@
         <v>90</v>
       </c>
       <c r="H217" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I217" s="1" t="s">
         <v>631</v>
@@ -46738,13 +46766,13 @@
         <v>669</v>
       </c>
       <c r="K217" s="1" t="s">
+        <v>2242</v>
+      </c>
+      <c r="L217" s="1" t="s">
         <v>2243</v>
       </c>
-      <c r="L217" s="1" t="s">
+      <c r="N217" s="1" t="s">
         <v>2244</v>
-      </c>
-      <c r="N217" s="1" t="s">
-        <v>2245</v>
       </c>
       <c r="O217" s="1" t="s">
         <v>97</v>
@@ -46843,13 +46871,13 @@
         <v>112</v>
       </c>
       <c r="BH217" s="1" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="BM217" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT217" s="1" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="BU217" s="1" t="s">
         <v>119</v>
@@ -46870,7 +46898,7 @@
         <v>98</v>
       </c>
       <c r="CC217" s="1" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="CD217" s="1" t="s">
         <v>667</v>
@@ -46884,10 +46912,10 @@
         <v>84</v>
       </c>
       <c r="B218" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>631</v>
@@ -46902,7 +46930,7 @@
         <v>90</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I218" s="1" t="s">
         <v>631</v>
@@ -46911,13 +46939,13 @@
         <v>669</v>
       </c>
       <c r="K218" s="1" t="s">
+        <v>2248</v>
+      </c>
+      <c r="L218" s="1" t="s">
+        <v>2165</v>
+      </c>
+      <c r="N218" s="1" t="s">
         <v>2249</v>
-      </c>
-      <c r="L218" s="1" t="s">
-        <v>2166</v>
-      </c>
-      <c r="N218" s="1" t="s">
-        <v>2250</v>
       </c>
       <c r="O218" s="1" t="s">
         <v>97</v>
@@ -47013,13 +47041,13 @@
         <v>112</v>
       </c>
       <c r="BH218" s="1" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
       <c r="BM218" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT218" s="1" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="BU218" s="1" t="s">
         <v>119</v>
@@ -47040,13 +47068,13 @@
         <v>98</v>
       </c>
       <c r="CC218" s="1" t="s">
+        <v>2252</v>
+      </c>
+      <c r="CD218" s="1" t="s">
         <v>2253</v>
       </c>
-      <c r="CD218" s="1" t="s">
+      <c r="CE218" s="1" t="s">
         <v>2254</v>
-      </c>
-      <c r="CE218" s="1" t="s">
-        <v>2255</v>
       </c>
     </row>
     <row r="219" spans="1:83" x14ac:dyDescent="0.25">
@@ -47054,10 +47082,10 @@
         <v>84</v>
       </c>
       <c r="B219" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>631</v>
@@ -47072,7 +47100,7 @@
         <v>90</v>
       </c>
       <c r="H219" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>631</v>
@@ -47081,13 +47109,13 @@
         <v>669</v>
       </c>
       <c r="K219" s="1" t="s">
+        <v>2255</v>
+      </c>
+      <c r="L219" s="1" t="s">
         <v>2256</v>
       </c>
-      <c r="L219" s="1" t="s">
+      <c r="N219" s="1" t="s">
         <v>2257</v>
-      </c>
-      <c r="N219" s="1" t="s">
-        <v>2258</v>
       </c>
       <c r="O219" s="1" t="s">
         <v>97</v>
@@ -47141,7 +47169,7 @@
         <v>0</v>
       </c>
       <c r="AN219" s="1" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="AO219" s="1">
         <v>0</v>
@@ -47186,13 +47214,13 @@
         <v>112</v>
       </c>
       <c r="BH219" s="1" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="BM219" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT219" s="1" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="BU219" s="1" t="s">
         <v>119</v>
@@ -47216,10 +47244,10 @@
         <v>1241</v>
       </c>
       <c r="CD219" s="1" t="s">
+        <v>2261</v>
+      </c>
+      <c r="CE219" s="1" t="s">
         <v>2262</v>
-      </c>
-      <c r="CE219" s="1" t="s">
-        <v>2263</v>
       </c>
     </row>
     <row r="220" spans="1:83" x14ac:dyDescent="0.25">
@@ -47227,10 +47255,10 @@
         <v>84</v>
       </c>
       <c r="B220" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>631</v>
@@ -47245,7 +47273,7 @@
         <v>90</v>
       </c>
       <c r="H220" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>631</v>
@@ -47254,13 +47282,13 @@
         <v>669</v>
       </c>
       <c r="K220" s="1" t="s">
+        <v>2263</v>
+      </c>
+      <c r="L220" s="1" t="s">
         <v>2264</v>
       </c>
-      <c r="L220" s="1" t="s">
+      <c r="N220" s="1" t="s">
         <v>2265</v>
-      </c>
-      <c r="N220" s="1" t="s">
-        <v>2266</v>
       </c>
       <c r="O220" s="1" t="s">
         <v>97</v>
@@ -47359,13 +47387,13 @@
         <v>112</v>
       </c>
       <c r="BH220" s="1" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="BM220" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT220" s="1" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
       <c r="BU220" s="1" t="s">
         <v>119</v>
@@ -47389,7 +47417,7 @@
         <v>1900</v>
       </c>
       <c r="CD220" s="1" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="CE220" s="1" t="s">
         <v>206</v>
@@ -47400,10 +47428,10 @@
         <v>84</v>
       </c>
       <c r="B221" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C221" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>631</v>
@@ -47418,7 +47446,7 @@
         <v>90</v>
       </c>
       <c r="H221" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I221" s="1" t="s">
         <v>631</v>
@@ -47427,13 +47455,13 @@
         <v>669</v>
       </c>
       <c r="K221" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="L221" s="1" t="s">
         <v>2270</v>
       </c>
-      <c r="L221" s="1" t="s">
+      <c r="N221" s="1" t="s">
         <v>2271</v>
-      </c>
-      <c r="N221" s="1" t="s">
-        <v>2272</v>
       </c>
       <c r="O221" s="1" t="s">
         <v>97</v>
@@ -47490,7 +47518,7 @@
         <v>0</v>
       </c>
       <c r="AN221" s="1" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
       <c r="AO221" s="1">
         <v>0</v>
@@ -47535,13 +47563,13 @@
         <v>112</v>
       </c>
       <c r="BH221" s="1" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="BM221" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT221" s="1" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
       <c r="BU221" s="1" t="s">
         <v>119</v>
@@ -47565,10 +47593,10 @@
         <v>557</v>
       </c>
       <c r="CD221" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="CE221" s="1" t="s">
         <v>2276</v>
-      </c>
-      <c r="CE221" s="1" t="s">
-        <v>2277</v>
       </c>
     </row>
     <row r="222" spans="1:83" x14ac:dyDescent="0.25">
@@ -47576,10 +47604,10 @@
         <v>84</v>
       </c>
       <c r="B222" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>631</v>
@@ -47594,7 +47622,7 @@
         <v>90</v>
       </c>
       <c r="H222" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I222" s="1" t="s">
         <v>631</v>
@@ -47603,13 +47631,13 @@
         <v>669</v>
       </c>
       <c r="K222" s="1" t="s">
+        <v>2277</v>
+      </c>
+      <c r="L222" s="1" t="s">
         <v>2278</v>
       </c>
-      <c r="L222" s="1" t="s">
+      <c r="N222" s="1" t="s">
         <v>2279</v>
-      </c>
-      <c r="N222" s="1" t="s">
-        <v>2280</v>
       </c>
       <c r="O222" s="1" t="s">
         <v>97</v>
@@ -47708,13 +47736,13 @@
         <v>112</v>
       </c>
       <c r="BH222" s="1" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="BM222" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT222" s="1" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
       <c r="BU222" s="1" t="s">
         <v>119</v>
@@ -47735,13 +47763,13 @@
         <v>98</v>
       </c>
       <c r="CC222" s="1" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="CD222" s="1" t="s">
         <v>686</v>
       </c>
       <c r="CE222" s="1" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="223" spans="1:83" x14ac:dyDescent="0.25">
@@ -47749,10 +47777,10 @@
         <v>84</v>
       </c>
       <c r="B223" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>631</v>
@@ -47767,7 +47795,7 @@
         <v>90</v>
       </c>
       <c r="H223" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I223" s="1" t="s">
         <v>631</v>
@@ -47776,13 +47804,13 @@
         <v>669</v>
       </c>
       <c r="K223" s="1" t="s">
+        <v>2284</v>
+      </c>
+      <c r="L223" s="1" t="s">
         <v>2285</v>
       </c>
-      <c r="L223" s="1" t="s">
+      <c r="N223" s="1" t="s">
         <v>2286</v>
-      </c>
-      <c r="N223" s="1" t="s">
-        <v>2287</v>
       </c>
       <c r="O223" s="1" t="s">
         <v>97</v>
@@ -47839,7 +47867,7 @@
         <v>0</v>
       </c>
       <c r="AN223" s="1" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="AO223" s="1">
         <v>0</v>
@@ -47884,13 +47912,13 @@
         <v>112</v>
       </c>
       <c r="BH223" s="1" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="BM223" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT223" s="1" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="BU223" s="1" t="s">
         <v>119</v>
@@ -47911,13 +47939,13 @@
         <v>98</v>
       </c>
       <c r="CC223" s="1" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="CD223" s="1" t="s">
         <v>1028</v>
       </c>
       <c r="CE223" s="1" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="224" spans="1:83" x14ac:dyDescent="0.25">
@@ -47925,10 +47953,10 @@
         <v>84</v>
       </c>
       <c r="B224" s="1" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C224" s="1" t="s">
         <v>2206</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>2207</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>631</v>
@@ -47943,7 +47971,7 @@
         <v>90</v>
       </c>
       <c r="H224" s="1" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="I224" s="1" t="s">
         <v>631</v>
@@ -47952,16 +47980,16 @@
         <v>669</v>
       </c>
       <c r="K224" s="1" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L224" s="1" t="s">
         <v>2293</v>
-      </c>
-      <c r="L224" s="1" t="s">
-        <v>2294</v>
       </c>
       <c r="M224" s="1" t="s">
         <v>108</v>
       </c>
       <c r="N224" s="1" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="O224" s="1" t="s">
         <v>97</v>
@@ -48060,13 +48088,13 @@
         <v>112</v>
       </c>
       <c r="BH224" s="1" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="BM224" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BT224" s="1" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="BU224" s="1" t="s">
         <v>119</v>
@@ -48087,16 +48115,17 @@
         <v>98</v>
       </c>
       <c r="CC224" s="1" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="CD224" s="1" t="s">
+        <v>2297</v>
+      </c>
+      <c r="CE224" s="1" t="s">
         <v>2298</v>
-      </c>
-      <c r="CE224" s="1" t="s">
-        <v>2299</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:CF224" xr:uid="{3AF25794-05F9-48DF-B327-7E0E0CFA0389}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>